<commit_message>
modelando estacionareidad de variables
</commit_message>
<xml_diff>
--- a/data/predicción_precios_fertilizantes.xlsx
+++ b/data/predicción_precios_fertilizantes.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>index</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>fob_urea_kg</t>
   </si>
@@ -31,7 +28,7 @@
     <t>inflación_mensual</t>
   </si>
   <si>
-    <t>diesel</t>
+    <t>ipc_diesel</t>
   </si>
   <si>
     <t>precipitación_media_mm</t>
@@ -40,7 +37,7 @@
     <t>temp_media_Celsius</t>
   </si>
   <si>
-    <t>otros_prod_agrícolas_exportados</t>
+    <t>fob_otros_prod_agrícolas_exportados_usd</t>
   </si>
   <si>
     <t>fosfato diamónico 18-46-0</t>
@@ -116,7 +113,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,41 +417,38 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12">

</xml_diff>